<commit_message>
finished std clean function and cleared duplicate marcelo problem
</commit_message>
<xml_diff>
--- a/data/league_data/france/20/france_std.xlsx
+++ b/data/league_data/france/20/france_std.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjitvarma/Desktop/trial_git/Predicting-Football-Player-Transfer-Values/data/league_data/france/20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45014A9D-7AB6-094B-BA5A-7F7C42754902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD9D05-2A0C-BB45-BF9C-20CD0A53EB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -637,9 +637,6 @@
     <t>Mounir Chouiar</t>
   </si>
   <si>
-    <t>Marcelo</t>
-  </si>
-  <si>
     <t>Mohamed Simakan</t>
   </si>
   <si>
@@ -1604,12 +1601,15 @@
   </si>
   <si>
     <t>Edmilson Indjai</t>
+  </si>
+  <si>
+    <t>Marcelo Filho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2470,11 +2470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG1" activeCellId="5" sqref="A1:A1048576 C1:C1048576 D1:D1048576 F1:F1048576 G1:G1048576 AG1:AG1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16283,7 +16283,7 @@
     </row>
     <row r="167" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>205</v>
+        <v>527</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>60</v>
@@ -16366,7 +16366,7 @@
     </row>
     <row r="168" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>47</v>
@@ -16449,7 +16449,7 @@
     </row>
     <row r="169" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>47</v>
@@ -16532,7 +16532,7 @@
     </row>
     <row r="170" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>51</v>
@@ -16615,7 +16615,7 @@
     </row>
     <row r="171" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>47</v>
@@ -16698,7 +16698,7 @@
     </row>
     <row r="172" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>25</v>
@@ -16781,7 +16781,7 @@
     </row>
     <row r="173" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>33</v>
@@ -16864,7 +16864,7 @@
     </row>
     <row r="174" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>116</v>
@@ -16947,7 +16947,7 @@
     </row>
     <row r="175" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>47</v>
@@ -17030,7 +17030,7 @@
     </row>
     <row r="176" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>116</v>
@@ -17113,7 +17113,7 @@
     </row>
     <row r="177" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>109</v>
@@ -17196,7 +17196,7 @@
     </row>
     <row r="178" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>51</v>
@@ -17279,7 +17279,7 @@
     </row>
     <row r="179" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>44</v>
@@ -17362,7 +17362,7 @@
     </row>
     <row r="180" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>57</v>
@@ -17445,7 +17445,7 @@
     </row>
     <row r="181" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>51</v>
@@ -17528,7 +17528,7 @@
     </row>
     <row r="182" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>27</v>
@@ -17611,7 +17611,7 @@
     </row>
     <row r="183" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>57</v>
@@ -17694,7 +17694,7 @@
     </row>
     <row r="184" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>33</v>
@@ -17777,7 +17777,7 @@
     </row>
     <row r="185" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>31</v>
@@ -17860,7 +17860,7 @@
     </row>
     <row r="186" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>55</v>
@@ -17943,7 +17943,7 @@
     </row>
     <row r="187" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>62</v>
@@ -18026,7 +18026,7 @@
     </row>
     <row r="188" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>51</v>
@@ -18109,7 +18109,7 @@
     </row>
     <row r="189" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>27</v>
@@ -18192,7 +18192,7 @@
     </row>
     <row r="190" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>21</v>
@@ -18275,7 +18275,7 @@
     </row>
     <row r="191" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>116</v>
@@ -18358,7 +18358,7 @@
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>35</v>
@@ -18441,7 +18441,7 @@
     </row>
     <row r="193" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>27</v>
@@ -18524,7 +18524,7 @@
     </row>
     <row r="194" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>62</v>
@@ -18607,7 +18607,7 @@
     </row>
     <row r="195" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>37</v>
@@ -18690,7 +18690,7 @@
     </row>
     <row r="196" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>35</v>
@@ -18773,7 +18773,7 @@
     </row>
     <row r="197" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>29</v>
@@ -18856,7 +18856,7 @@
     </row>
     <row r="198" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>25</v>
@@ -18939,7 +18939,7 @@
     </row>
     <row r="199" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>60</v>
@@ -19022,7 +19022,7 @@
     </row>
     <row r="200" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>55</v>
@@ -19105,7 +19105,7 @@
     </row>
     <row r="201" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>23</v>
@@ -19188,7 +19188,7 @@
     </row>
     <row r="202" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>60</v>
@@ -19271,7 +19271,7 @@
     </row>
     <row r="203" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>62</v>
@@ -19354,7 +19354,7 @@
     </row>
     <row r="204" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>21</v>
@@ -19437,7 +19437,7 @@
     </row>
     <row r="205" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>116</v>
@@ -19520,7 +19520,7 @@
     </row>
     <row r="206" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>109</v>
@@ -19603,7 +19603,7 @@
     </row>
     <row r="207" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>31</v>
@@ -19686,7 +19686,7 @@
     </row>
     <row r="208" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>39</v>
@@ -19769,7 +19769,7 @@
     </row>
     <row r="209" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>49</v>
@@ -19852,7 +19852,7 @@
     </row>
     <row r="210" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>51</v>
@@ -19935,7 +19935,7 @@
     </row>
     <row r="211" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>47</v>
@@ -20018,7 +20018,7 @@
     </row>
     <row r="212" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>116</v>
@@ -20101,7 +20101,7 @@
     </row>
     <row r="213" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>57</v>
@@ -20184,7 +20184,7 @@
     </row>
     <row r="214" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>35</v>
@@ -20267,7 +20267,7 @@
     </row>
     <row r="215" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>37</v>
@@ -20350,7 +20350,7 @@
     </row>
     <row r="216" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>23</v>
@@ -20433,7 +20433,7 @@
     </row>
     <row r="217" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>60</v>
@@ -20516,7 +20516,7 @@
     </row>
     <row r="218" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>49</v>
@@ -20599,7 +20599,7 @@
     </row>
     <row r="219" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>57</v>
@@ -20682,7 +20682,7 @@
     </row>
     <row r="220" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>116</v>
@@ -20765,7 +20765,7 @@
     </row>
     <row r="221" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>51</v>
@@ -20848,7 +20848,7 @@
     </row>
     <row r="222" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>116</v>
@@ -20931,7 +20931,7 @@
     </row>
     <row r="223" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>51</v>
@@ -21014,7 +21014,7 @@
     </row>
     <row r="224" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>31</v>
@@ -21097,7 +21097,7 @@
     </row>
     <row r="225" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>109</v>
@@ -21180,7 +21180,7 @@
     </row>
     <row r="226" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>33</v>
@@ -21263,7 +21263,7 @@
     </row>
     <row r="227" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>29</v>
@@ -21346,7 +21346,7 @@
     </row>
     <row r="228" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>49</v>
@@ -21429,7 +21429,7 @@
     </row>
     <row r="229" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>116</v>
@@ -21512,7 +21512,7 @@
     </row>
     <row r="230" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>60</v>
@@ -21595,7 +21595,7 @@
     </row>
     <row r="231" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>29</v>
@@ -21678,7 +21678,7 @@
     </row>
     <row r="232" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>51</v>
@@ -21761,7 +21761,7 @@
     </row>
     <row r="233" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>35</v>
@@ -21844,7 +21844,7 @@
     </row>
     <row r="234" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>116</v>
@@ -21927,7 +21927,7 @@
     </row>
     <row r="235" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>62</v>
@@ -22010,7 +22010,7 @@
     </row>
     <row r="236" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>37</v>
@@ -22093,7 +22093,7 @@
     </row>
     <row r="237" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>109</v>
@@ -22176,7 +22176,7 @@
     </row>
     <row r="238" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>35</v>
@@ -22259,7 +22259,7 @@
     </row>
     <row r="239" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>29</v>
@@ -22342,7 +22342,7 @@
     </row>
     <row r="240" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>57</v>
@@ -22425,7 +22425,7 @@
     </row>
     <row r="241" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>57</v>
@@ -22508,7 +22508,7 @@
     </row>
     <row r="242" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>57</v>
@@ -22591,7 +22591,7 @@
     </row>
     <row r="243" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>55</v>
@@ -22674,7 +22674,7 @@
     </row>
     <row r="244" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>33</v>
@@ -22757,7 +22757,7 @@
     </row>
     <row r="245" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>25</v>
@@ -22840,7 +22840,7 @@
     </row>
     <row r="246" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>29</v>
@@ -22923,7 +22923,7 @@
     </row>
     <row r="247" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>23</v>
@@ -23006,7 +23006,7 @@
     </row>
     <row r="248" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>49</v>
@@ -23089,7 +23089,7 @@
     </row>
     <row r="249" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>109</v>
@@ -23172,7 +23172,7 @@
     </row>
     <row r="250" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>31</v>
@@ -23255,7 +23255,7 @@
     </row>
     <row r="251" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>60</v>
@@ -23338,7 +23338,7 @@
     </row>
     <row r="252" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>31</v>
@@ -23421,7 +23421,7 @@
     </row>
     <row r="253" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>31</v>
@@ -23504,7 +23504,7 @@
     </row>
     <row r="254" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>47</v>
@@ -23587,7 +23587,7 @@
     </row>
     <row r="255" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>23</v>
@@ -23670,7 +23670,7 @@
     </row>
     <row r="256" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>25</v>
@@ -23753,7 +23753,7 @@
     </row>
     <row r="257" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>60</v>
@@ -23836,7 +23836,7 @@
     </row>
     <row r="258" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>47</v>
@@ -23919,7 +23919,7 @@
     </row>
     <row r="259" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>23</v>
@@ -24002,7 +24002,7 @@
     </row>
     <row r="260" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>57</v>
@@ -24085,7 +24085,7 @@
     </row>
     <row r="261" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>25</v>
@@ -24168,7 +24168,7 @@
     </row>
     <row r="262" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>35</v>
@@ -24251,7 +24251,7 @@
     </row>
     <row r="263" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>109</v>
@@ -24334,7 +24334,7 @@
     </row>
     <row r="264" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>109</v>
@@ -24417,7 +24417,7 @@
     </row>
     <row r="265" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>29</v>
@@ -24500,7 +24500,7 @@
     </row>
     <row r="266" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B266" s="3" t="s">
         <v>25</v>
@@ -24583,7 +24583,7 @@
     </row>
     <row r="267" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B267" s="3" t="s">
         <v>57</v>
@@ -24666,7 +24666,7 @@
     </row>
     <row r="268" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>33</v>
@@ -24749,7 +24749,7 @@
     </row>
     <row r="269" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B269" s="3" t="s">
         <v>27</v>
@@ -24832,7 +24832,7 @@
     </row>
     <row r="270" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B270" s="3" t="s">
         <v>23</v>
@@ -24915,7 +24915,7 @@
     </row>
     <row r="271" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B271" s="3" t="s">
         <v>21</v>
@@ -24998,7 +24998,7 @@
     </row>
     <row r="272" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B272" s="3" t="s">
         <v>31</v>
@@ -25081,7 +25081,7 @@
     </row>
     <row r="273" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B273" s="3" t="s">
         <v>49</v>
@@ -25164,7 +25164,7 @@
     </row>
     <row r="274" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>62</v>
@@ -25247,7 +25247,7 @@
     </row>
     <row r="275" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>39</v>
@@ -25330,7 +25330,7 @@
     </row>
     <row r="276" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B276" s="3" t="s">
         <v>109</v>
@@ -25413,7 +25413,7 @@
     </row>
     <row r="277" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B277" s="3" t="s">
         <v>25</v>
@@ -25496,7 +25496,7 @@
     </row>
     <row r="278" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B278" s="3" t="s">
         <v>35</v>
@@ -25579,7 +25579,7 @@
     </row>
     <row r="279" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B279" s="3" t="s">
         <v>27</v>
@@ -25662,7 +25662,7 @@
     </row>
     <row r="280" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>109</v>
@@ -25745,7 +25745,7 @@
     </row>
     <row r="281" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>51</v>
@@ -25828,7 +25828,7 @@
     </row>
     <row r="282" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>21</v>
@@ -25911,7 +25911,7 @@
     </row>
     <row r="283" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>31</v>
@@ -25994,7 +25994,7 @@
     </row>
     <row r="284" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>55</v>
@@ -26077,7 +26077,7 @@
     </row>
     <row r="285" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B285" s="3" t="s">
         <v>49</v>
@@ -26160,7 +26160,7 @@
     </row>
     <row r="286" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>35</v>
@@ -26243,7 +26243,7 @@
     </row>
     <row r="287" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>109</v>
@@ -26326,7 +26326,7 @@
     </row>
     <row r="288" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>31</v>
@@ -26409,7 +26409,7 @@
     </row>
     <row r="289" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>109</v>
@@ -26492,7 +26492,7 @@
     </row>
     <row r="290" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>29</v>
@@ -26575,7 +26575,7 @@
     </row>
     <row r="291" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>116</v>
@@ -26658,7 +26658,7 @@
     </row>
     <row r="292" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>35</v>
@@ -26741,7 +26741,7 @@
     </row>
     <row r="293" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B293" s="3" t="s">
         <v>109</v>
@@ -26824,7 +26824,7 @@
     </row>
     <row r="294" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B294" s="3" t="s">
         <v>29</v>
@@ -26907,7 +26907,7 @@
     </row>
     <row r="295" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B295" s="3" t="s">
         <v>33</v>
@@ -26990,7 +26990,7 @@
     </row>
     <row r="296" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B296" s="3" t="s">
         <v>44</v>
@@ -27073,7 +27073,7 @@
     </row>
     <row r="297" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B297" s="3" t="s">
         <v>49</v>
@@ -27156,7 +27156,7 @@
     </row>
     <row r="298" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B298" s="3" t="s">
         <v>21</v>
@@ -27239,7 +27239,7 @@
     </row>
     <row r="299" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>33</v>
@@ -27322,7 +27322,7 @@
     </row>
     <row r="300" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B300" s="3" t="s">
         <v>51</v>
@@ -27405,7 +27405,7 @@
     </row>
     <row r="301" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B301" s="3" t="s">
         <v>60</v>
@@ -27488,7 +27488,7 @@
     </row>
     <row r="302" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>23</v>
@@ -27571,7 +27571,7 @@
     </row>
     <row r="303" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B303" s="3" t="s">
         <v>51</v>
@@ -27654,7 +27654,7 @@
     </row>
     <row r="304" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B304" s="3" t="s">
         <v>60</v>
@@ -27737,7 +27737,7 @@
     </row>
     <row r="305" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>23</v>
@@ -27820,7 +27820,7 @@
     </row>
     <row r="306" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>116</v>
@@ -27903,7 +27903,7 @@
     </row>
     <row r="307" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>39</v>
@@ -27986,7 +27986,7 @@
     </row>
     <row r="308" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B308" s="3" t="s">
         <v>37</v>
@@ -28069,7 +28069,7 @@
     </row>
     <row r="309" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B309" s="3" t="s">
         <v>27</v>
@@ -28152,7 +28152,7 @@
     </row>
     <row r="310" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B310" s="3" t="s">
         <v>60</v>
@@ -28235,7 +28235,7 @@
     </row>
     <row r="311" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B311" s="3" t="s">
         <v>35</v>
@@ -28318,7 +28318,7 @@
     </row>
     <row r="312" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B312" s="3" t="s">
         <v>62</v>
@@ -28401,7 +28401,7 @@
     </row>
     <row r="313" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>23</v>
@@ -28484,7 +28484,7 @@
     </row>
     <row r="314" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B314" s="3" t="s">
         <v>57</v>
@@ -28567,7 +28567,7 @@
     </row>
     <row r="315" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B315" s="3" t="s">
         <v>25</v>
@@ -28650,7 +28650,7 @@
     </row>
     <row r="316" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B316" s="3" t="s">
         <v>33</v>
@@ -28733,7 +28733,7 @@
     </row>
     <row r="317" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B317" s="3" t="s">
         <v>60</v>
@@ -28816,7 +28816,7 @@
     </row>
     <row r="318" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B318" s="3" t="s">
         <v>47</v>
@@ -28899,7 +28899,7 @@
     </row>
     <row r="319" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>116</v>
@@ -28982,7 +28982,7 @@
     </row>
     <row r="320" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>39</v>
@@ -29065,7 +29065,7 @@
     </row>
     <row r="321" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>44</v>
@@ -29148,7 +29148,7 @@
     </row>
     <row r="322" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>57</v>
@@ -29231,7 +29231,7 @@
     </row>
     <row r="323" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B323" s="3" t="s">
         <v>27</v>
@@ -29314,7 +29314,7 @@
     </row>
     <row r="324" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>116</v>
@@ -29397,7 +29397,7 @@
     </row>
     <row r="325" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B325" s="3" t="s">
         <v>109</v>
@@ -29480,7 +29480,7 @@
     </row>
     <row r="326" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B326" s="3" t="s">
         <v>33</v>
@@ -29563,7 +29563,7 @@
     </row>
     <row r="327" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B327" s="3" t="s">
         <v>35</v>
@@ -29646,7 +29646,7 @@
     </row>
     <row r="328" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B328" s="3" t="s">
         <v>39</v>
@@ -29729,7 +29729,7 @@
     </row>
     <row r="329" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B329" s="3" t="s">
         <v>57</v>
@@ -29812,7 +29812,7 @@
     </row>
     <row r="330" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B330" s="3" t="s">
         <v>25</v>
@@ -29895,7 +29895,7 @@
     </row>
     <row r="331" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B331" s="3" t="s">
         <v>109</v>
@@ -29978,7 +29978,7 @@
     </row>
     <row r="332" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B332" s="3" t="s">
         <v>29</v>
@@ -30061,7 +30061,7 @@
     </row>
     <row r="333" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B333" s="3" t="s">
         <v>109</v>
@@ -30144,7 +30144,7 @@
     </row>
     <row r="334" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B334" s="3" t="s">
         <v>21</v>
@@ -30227,7 +30227,7 @@
     </row>
     <row r="335" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B335" s="3" t="s">
         <v>31</v>
@@ -30310,7 +30310,7 @@
     </row>
     <row r="336" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B336" s="3" t="s">
         <v>29</v>
@@ -30393,7 +30393,7 @@
     </row>
     <row r="337" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B337" s="3" t="s">
         <v>116</v>
@@ -30476,7 +30476,7 @@
     </row>
     <row r="338" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B338" s="3" t="s">
         <v>62</v>
@@ -30559,7 +30559,7 @@
     </row>
     <row r="339" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B339" s="3" t="s">
         <v>21</v>
@@ -30642,7 +30642,7 @@
     </row>
     <row r="340" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B340" s="3" t="s">
         <v>57</v>
@@ -30725,7 +30725,7 @@
     </row>
     <row r="341" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B341" s="3" t="s">
         <v>62</v>
@@ -30808,7 +30808,7 @@
     </row>
     <row r="342" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B342" s="3" t="s">
         <v>37</v>
@@ -30891,7 +30891,7 @@
     </row>
     <row r="343" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B343" s="3" t="s">
         <v>51</v>
@@ -30974,7 +30974,7 @@
     </row>
     <row r="344" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B344" s="3" t="s">
         <v>25</v>
@@ -31057,7 +31057,7 @@
     </row>
     <row r="345" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B345" s="3" t="s">
         <v>60</v>
@@ -31140,7 +31140,7 @@
     </row>
     <row r="346" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B346" s="3" t="s">
         <v>39</v>
@@ -31223,7 +31223,7 @@
     </row>
     <row r="347" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B347" s="3" t="s">
         <v>37</v>
@@ -31306,7 +31306,7 @@
     </row>
     <row r="348" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B348" s="3" t="s">
         <v>25</v>
@@ -31389,7 +31389,7 @@
     </row>
     <row r="349" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B349" s="3" t="s">
         <v>23</v>
@@ -31472,7 +31472,7 @@
     </row>
     <row r="350" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B350" s="3" t="s">
         <v>116</v>
@@ -31555,7 +31555,7 @@
     </row>
     <row r="351" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B351" s="3" t="s">
         <v>25</v>
@@ -31638,7 +31638,7 @@
     </row>
     <row r="352" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>29</v>
@@ -31721,7 +31721,7 @@
     </row>
     <row r="353" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B353" s="3" t="s">
         <v>27</v>
@@ -31804,7 +31804,7 @@
     </row>
     <row r="354" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B354" s="3" t="s">
         <v>60</v>
@@ -31887,7 +31887,7 @@
     </row>
     <row r="355" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B355" s="3" t="s">
         <v>47</v>
@@ -31970,7 +31970,7 @@
     </row>
     <row r="356" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>21</v>
@@ -32053,7 +32053,7 @@
     </row>
     <row r="357" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>47</v>
@@ -32136,7 +32136,7 @@
     </row>
     <row r="358" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>62</v>
@@ -32219,7 +32219,7 @@
     </row>
     <row r="359" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>44</v>
@@ -32302,7 +32302,7 @@
     </row>
     <row r="360" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>23</v>
@@ -32385,7 +32385,7 @@
     </row>
     <row r="361" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>27</v>
@@ -32468,7 +32468,7 @@
     </row>
     <row r="362" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>57</v>
@@ -32551,7 +32551,7 @@
     </row>
     <row r="363" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B363" s="3" t="s">
         <v>57</v>
@@ -32634,7 +32634,7 @@
     </row>
     <row r="364" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>31</v>
@@ -32717,7 +32717,7 @@
     </row>
     <row r="365" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B365" s="3" t="s">
         <v>116</v>
@@ -32800,7 +32800,7 @@
     </row>
     <row r="366" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B366" s="3" t="s">
         <v>23</v>
@@ -32883,7 +32883,7 @@
     </row>
     <row r="367" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B367" s="3" t="s">
         <v>109</v>
@@ -32966,7 +32966,7 @@
     </row>
     <row r="368" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>27</v>
@@ -33049,7 +33049,7 @@
     </row>
     <row r="369" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B369" s="3" t="s">
         <v>39</v>
@@ -33132,7 +33132,7 @@
     </row>
     <row r="370" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>21</v>
@@ -33215,7 +33215,7 @@
     </row>
     <row r="371" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B371" s="3" t="s">
         <v>39</v>
@@ -33298,7 +33298,7 @@
     </row>
     <row r="372" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B372" s="3" t="s">
         <v>116</v>
@@ -33381,7 +33381,7 @@
     </row>
     <row r="373" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B373" s="3" t="s">
         <v>116</v>
@@ -33464,7 +33464,7 @@
     </row>
     <row r="374" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B374" s="3" t="s">
         <v>109</v>
@@ -33547,7 +33547,7 @@
     </row>
     <row r="375" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B375" s="3" t="s">
         <v>33</v>
@@ -33630,7 +33630,7 @@
     </row>
     <row r="376" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B376" s="3" t="s">
         <v>49</v>
@@ -33713,7 +33713,7 @@
     </row>
     <row r="377" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B377" s="3" t="s">
         <v>44</v>
@@ -33796,7 +33796,7 @@
     </row>
     <row r="378" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B378" s="3" t="s">
         <v>109</v>
@@ -33879,7 +33879,7 @@
     </row>
     <row r="379" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B379" s="3" t="s">
         <v>33</v>
@@ -33962,7 +33962,7 @@
     </row>
     <row r="380" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B380" s="3" t="s">
         <v>27</v>
@@ -34045,7 +34045,7 @@
     </row>
     <row r="381" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B381" s="3" t="s">
         <v>21</v>
@@ -34128,7 +34128,7 @@
     </row>
     <row r="382" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B382" s="3" t="s">
         <v>49</v>
@@ -34211,7 +34211,7 @@
     </row>
     <row r="383" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B383" s="3" t="s">
         <v>27</v>
@@ -34294,7 +34294,7 @@
     </row>
     <row r="384" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B384" s="3" t="s">
         <v>47</v>
@@ -34377,7 +34377,7 @@
     </row>
     <row r="385" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B385" s="3" t="s">
         <v>47</v>
@@ -34460,7 +34460,7 @@
     </row>
     <row r="386" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B386" s="3" t="s">
         <v>55</v>
@@ -34543,7 +34543,7 @@
     </row>
     <row r="387" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B387" s="3" t="s">
         <v>49</v>
@@ -34626,7 +34626,7 @@
     </row>
     <row r="388" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B388" s="3" t="s">
         <v>44</v>
@@ -34709,7 +34709,7 @@
     </row>
     <row r="389" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B389" s="3" t="s">
         <v>29</v>
@@ -34792,7 +34792,7 @@
     </row>
     <row r="390" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B390" s="3" t="s">
         <v>44</v>
@@ -34875,7 +34875,7 @@
     </row>
     <row r="391" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B391" s="3" t="s">
         <v>62</v>
@@ -34958,7 +34958,7 @@
     </row>
     <row r="392" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B392" s="3" t="s">
         <v>35</v>
@@ -35041,7 +35041,7 @@
     </row>
     <row r="393" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B393" s="3" t="s">
         <v>35</v>
@@ -35124,7 +35124,7 @@
     </row>
     <row r="394" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B394" s="3" t="s">
         <v>39</v>
@@ -35207,7 +35207,7 @@
     </row>
     <row r="395" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B395" s="3" t="s">
         <v>44</v>
@@ -35290,7 +35290,7 @@
     </row>
     <row r="396" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A396" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B396" s="3" t="s">
         <v>116</v>
@@ -35373,7 +35373,7 @@
     </row>
     <row r="397" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B397" s="3" t="s">
         <v>31</v>
@@ -35456,7 +35456,7 @@
     </row>
     <row r="398" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A398" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B398" s="3" t="s">
         <v>23</v>
@@ -35539,7 +35539,7 @@
     </row>
     <row r="399" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B399" s="3" t="s">
         <v>29</v>
@@ -35622,7 +35622,7 @@
     </row>
     <row r="400" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A400" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B400" s="3" t="s">
         <v>60</v>
@@ -35705,7 +35705,7 @@
     </row>
     <row r="401" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B401" s="3" t="s">
         <v>44</v>
@@ -35788,7 +35788,7 @@
     </row>
     <row r="402" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A402" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B402" s="3" t="s">
         <v>57</v>
@@ -35954,7 +35954,7 @@
     </row>
     <row r="404" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B404" s="3" t="s">
         <v>47</v>
@@ -36037,7 +36037,7 @@
     </row>
     <row r="405" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B405" s="3" t="s">
         <v>21</v>
@@ -36120,7 +36120,7 @@
     </row>
     <row r="406" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A406" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B406" s="3" t="s">
         <v>47</v>
@@ -36203,7 +36203,7 @@
     </row>
     <row r="407" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B407" s="3" t="s">
         <v>29</v>
@@ -36286,7 +36286,7 @@
     </row>
     <row r="408" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B408" s="3" t="s">
         <v>51</v>
@@ -36369,7 +36369,7 @@
     </row>
     <row r="409" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B409" s="3" t="s">
         <v>109</v>
@@ -36452,7 +36452,7 @@
     </row>
     <row r="410" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B410" s="3" t="s">
         <v>49</v>
@@ -36535,7 +36535,7 @@
     </row>
     <row r="411" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B411" s="3" t="s">
         <v>37</v>
@@ -36618,7 +36618,7 @@
     </row>
     <row r="412" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B412" s="3" t="s">
         <v>25</v>
@@ -36701,7 +36701,7 @@
     </row>
     <row r="413" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B413" s="3" t="s">
         <v>60</v>
@@ -36784,7 +36784,7 @@
     </row>
     <row r="414" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A414" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B414" s="3" t="s">
         <v>27</v>
@@ -36867,7 +36867,7 @@
     </row>
     <row r="415" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B415" s="3" t="s">
         <v>57</v>
@@ -36950,7 +36950,7 @@
     </row>
     <row r="416" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A416" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B416" s="3" t="s">
         <v>55</v>
@@ -37033,7 +37033,7 @@
     </row>
     <row r="417" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A417" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B417" s="3" t="s">
         <v>27</v>
@@ -37116,7 +37116,7 @@
     </row>
     <row r="418" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A418" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B418" s="3" t="s">
         <v>25</v>
@@ -37199,7 +37199,7 @@
     </row>
     <row r="419" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A419" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B419" s="3" t="s">
         <v>44</v>
@@ -37282,7 +37282,7 @@
     </row>
     <row r="420" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A420" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B420" s="3" t="s">
         <v>62</v>
@@ -37365,7 +37365,7 @@
     </row>
     <row r="421" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A421" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B421" s="3" t="s">
         <v>57</v>
@@ -37448,7 +37448,7 @@
     </row>
     <row r="422" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A422" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B422" s="3" t="s">
         <v>35</v>
@@ -37531,7 +37531,7 @@
     </row>
     <row r="423" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B423" s="3" t="s">
         <v>39</v>
@@ -37614,7 +37614,7 @@
     </row>
     <row r="424" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A424" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B424" s="3" t="s">
         <v>116</v>
@@ -37697,7 +37697,7 @@
     </row>
     <row r="425" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B425" s="3" t="s">
         <v>60</v>
@@ -37780,7 +37780,7 @@
     </row>
     <row r="426" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A426" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B426" s="3" t="s">
         <v>25</v>
@@ -37863,7 +37863,7 @@
     </row>
     <row r="427" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B427" s="3" t="s">
         <v>27</v>
@@ -37946,7 +37946,7 @@
     </row>
     <row r="428" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A428" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B428" s="3" t="s">
         <v>49</v>
@@ -38029,7 +38029,7 @@
     </row>
     <row r="429" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B429" s="3" t="s">
         <v>27</v>
@@ -38112,7 +38112,7 @@
     </row>
     <row r="430" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A430" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B430" s="3" t="s">
         <v>37</v>
@@ -38195,7 +38195,7 @@
     </row>
     <row r="431" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B431" s="3" t="s">
         <v>57</v>
@@ -38278,7 +38278,7 @@
     </row>
     <row r="432" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A432" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B432" s="3" t="s">
         <v>27</v>
@@ -38361,7 +38361,7 @@
     </row>
     <row r="433" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B433" s="3" t="s">
         <v>31</v>
@@ -38444,7 +38444,7 @@
     </row>
     <row r="434" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B434" s="3" t="s">
         <v>44</v>
@@ -38527,7 +38527,7 @@
     </row>
     <row r="435" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B435" s="3" t="s">
         <v>44</v>
@@ -38610,7 +38610,7 @@
     </row>
     <row r="436" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B436" s="3" t="s">
         <v>55</v>
@@ -38693,7 +38693,7 @@
     </row>
     <row r="437" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B437" s="3" t="s">
         <v>37</v>
@@ -38776,7 +38776,7 @@
     </row>
     <row r="438" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A438" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B438" s="3" t="s">
         <v>60</v>
@@ -38859,7 +38859,7 @@
     </row>
     <row r="439" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B439" s="3" t="s">
         <v>37</v>
@@ -38942,7 +38942,7 @@
     </row>
     <row r="440" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A440" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B440" s="3" t="s">
         <v>62</v>
@@ -39025,7 +39025,7 @@
     </row>
     <row r="441" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B441" s="3" t="s">
         <v>51</v>
@@ -39108,7 +39108,7 @@
     </row>
     <row r="442" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B442" s="3" t="s">
         <v>21</v>
@@ -39191,7 +39191,7 @@
     </row>
     <row r="443" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B443" s="3" t="s">
         <v>57</v>
@@ -39274,7 +39274,7 @@
     </row>
     <row r="444" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B444" s="3" t="s">
         <v>109</v>
@@ -39357,7 +39357,7 @@
     </row>
     <row r="445" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B445" s="3" t="s">
         <v>23</v>
@@ -39440,7 +39440,7 @@
     </row>
     <row r="446" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B446" s="3" t="s">
         <v>57</v>
@@ -39523,7 +39523,7 @@
     </row>
     <row r="447" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B447" s="3" t="s">
         <v>31</v>
@@ -39606,7 +39606,7 @@
     </row>
     <row r="448" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B448" s="3" t="s">
         <v>51</v>
@@ -39689,7 +39689,7 @@
     </row>
     <row r="449" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B449" s="3" t="s">
         <v>62</v>
@@ -39772,7 +39772,7 @@
     </row>
     <row r="450" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A450" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B450" s="3" t="s">
         <v>62</v>
@@ -39855,7 +39855,7 @@
     </row>
     <row r="451" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B451" s="3" t="s">
         <v>109</v>
@@ -39938,7 +39938,7 @@
     </row>
     <row r="452" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A452" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B452" s="3" t="s">
         <v>37</v>
@@ -40021,7 +40021,7 @@
     </row>
     <row r="453" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B453" s="3" t="s">
         <v>49</v>
@@ -40104,7 +40104,7 @@
     </row>
     <row r="454" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A454" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B454" s="3" t="s">
         <v>49</v>
@@ -40187,7 +40187,7 @@
     </row>
     <row r="455" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B455" s="3" t="s">
         <v>39</v>
@@ -40270,7 +40270,7 @@
     </row>
     <row r="456" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A456" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B456" s="3" t="s">
         <v>29</v>
@@ -40353,7 +40353,7 @@
     </row>
     <row r="457" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B457" s="3" t="s">
         <v>55</v>
@@ -40436,7 +40436,7 @@
     </row>
     <row r="458" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A458" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B458" s="3" t="s">
         <v>31</v>
@@ -40519,7 +40519,7 @@
     </row>
     <row r="459" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B459" s="3" t="s">
         <v>37</v>
@@ -40602,7 +40602,7 @@
     </row>
     <row r="460" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A460" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B460" s="3" t="s">
         <v>55</v>
@@ -40685,7 +40685,7 @@
     </row>
     <row r="461" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B461" s="3" t="s">
         <v>57</v>
@@ -40768,7 +40768,7 @@
     </row>
     <row r="462" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A462" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B462" s="3" t="s">
         <v>109</v>
@@ -40851,7 +40851,7 @@
     </row>
     <row r="463" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B463" s="3" t="s">
         <v>109</v>
@@ -40934,7 +40934,7 @@
     </row>
     <row r="464" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A464" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B464" s="3" t="s">
         <v>116</v>
@@ -41017,7 +41017,7 @@
     </row>
     <row r="465" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B465" s="3" t="s">
         <v>29</v>
@@ -41100,7 +41100,7 @@
     </row>
     <row r="466" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A466" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B466" s="3" t="s">
         <v>116</v>
@@ -41183,7 +41183,7 @@
     </row>
     <row r="467" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B467" s="3" t="s">
         <v>35</v>
@@ -41266,7 +41266,7 @@
     </row>
     <row r="468" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A468" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B468" s="3" t="s">
         <v>49</v>
@@ -41349,7 +41349,7 @@
     </row>
     <row r="469" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B469" s="3" t="s">
         <v>21</v>
@@ -41432,7 +41432,7 @@
     </row>
     <row r="470" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A470" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B470" s="3" t="s">
         <v>21</v>
@@ -41515,7 +41515,7 @@
     </row>
     <row r="471" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B471" s="3" t="s">
         <v>44</v>
@@ -41598,7 +41598,7 @@
     </row>
     <row r="472" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A472" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B472" s="3" t="s">
         <v>35</v>
@@ -41681,7 +41681,7 @@
     </row>
     <row r="473" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B473" s="3" t="s">
         <v>62</v>
@@ -41764,7 +41764,7 @@
     </row>
     <row r="474" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A474" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B474" s="3" t="s">
         <v>37</v>
@@ -41847,7 +41847,7 @@
     </row>
     <row r="475" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A475" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B475" s="3" t="s">
         <v>31</v>
@@ -41930,7 +41930,7 @@
     </row>
     <row r="476" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A476" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B476" s="3" t="s">
         <v>29</v>
@@ -42013,7 +42013,7 @@
     </row>
     <row r="477" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A477" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B477" s="3" t="s">
         <v>33</v>
@@ -42096,7 +42096,7 @@
     </row>
     <row r="478" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A478" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B478" s="3" t="s">
         <v>47</v>
@@ -42179,7 +42179,7 @@
     </row>
     <row r="479" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A479" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B479" s="3" t="s">
         <v>39</v>
@@ -42262,7 +42262,7 @@
     </row>
     <row r="480" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A480" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B480" s="3" t="s">
         <v>33</v>
@@ -42345,7 +42345,7 @@
     </row>
     <row r="481" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A481" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B481" s="3" t="s">
         <v>37</v>
@@ -42428,7 +42428,7 @@
     </row>
     <row r="482" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A482" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B482" s="3" t="s">
         <v>49</v>
@@ -42511,7 +42511,7 @@
     </row>
     <row r="483" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A483" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B483" s="3" t="s">
         <v>39</v>
@@ -42594,7 +42594,7 @@
     </row>
     <row r="484" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A484" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B484" s="3" t="s">
         <v>62</v>
@@ -42677,7 +42677,7 @@
     </row>
     <row r="485" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A485" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B485" s="3" t="s">
         <v>116</v>
@@ -42760,7 +42760,7 @@
     </row>
     <row r="486" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A486" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B486" s="3" t="s">
         <v>25</v>
@@ -42843,7 +42843,7 @@
     </row>
     <row r="487" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A487" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B487" s="3" t="s">
         <v>39</v>
@@ -42926,7 +42926,7 @@
     </row>
     <row r="488" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A488" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B488" s="3" t="s">
         <v>31</v>
@@ -43009,7 +43009,7 @@
     </row>
     <row r="489" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A489" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B489" s="3" t="s">
         <v>39</v>
@@ -43092,7 +43092,7 @@
     </row>
     <row r="490" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A490" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B490" s="3" t="s">
         <v>37</v>
@@ -43175,7 +43175,7 @@
     </row>
     <row r="491" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A491" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B491" s="3" t="s">
         <v>31</v>
@@ -43258,7 +43258,7 @@
     </row>
     <row r="492" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A492" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B492" s="3" t="s">
         <v>57</v>
@@ -43341,7 +43341,7 @@
     </row>
     <row r="493" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A493" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B493" s="3" t="s">
         <v>33</v>
@@ -43424,7 +43424,7 @@
     </row>
     <row r="494" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A494" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B494" s="3" t="s">
         <v>116</v>
@@ -43507,7 +43507,7 @@
     </row>
     <row r="495" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A495" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B495" s="3" t="s">
         <v>27</v>
@@ -43572,7 +43572,7 @@
     </row>
     <row r="496" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A496" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B496" s="3" t="s">
         <v>57</v>
@@ -43655,7 +43655,7 @@
     </row>
     <row r="497" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A497" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B497" s="3" t="s">
         <v>35</v>
@@ -43738,7 +43738,7 @@
     </row>
     <row r="498" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A498" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B498" s="3" t="s">
         <v>60</v>
@@ -43821,7 +43821,7 @@
     </row>
     <row r="499" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A499" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B499" s="3" t="s">
         <v>44</v>
@@ -43904,7 +43904,7 @@
     </row>
     <row r="500" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A500" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B500" s="3" t="s">
         <v>109</v>

</xml_diff>